<commit_message>
Corregimos inscripciones de ninacos
</commit_message>
<xml_diff>
--- a/ayudas/costos de guarderia.xlsx
+++ b/ayudas/costos de guarderia.xlsx
@@ -766,7 +766,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.000000000000000"/>
-    <numFmt numFmtId="178" formatCode="#,##0.00000000000000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00000000000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -852,7 +852,7 @@
     <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1141,8 +1141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E2:L255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="E108" sqref="E108:I108"/>
+    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1397,7 +1397,10 @@
         <f t="shared" si="1"/>
         <v>182.05211169927236</v>
       </c>
-      <c r="I16" s="1"/>
+      <c r="I16" s="1" t="e">
+        <f>I15*J16/J15</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="17" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E17" s="5">

</xml_diff>